<commit_message>
button to dowloadCsv on import
</commit_message>
<xml_diff>
--- a/frontend/src/assets/data/User_CompanyExample.xlsx
+++ b/frontend/src/assets/data/User_CompanyExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projeto\surf-management-app\frontend\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C9F67B-CEE4-4FE6-9591-1C764BC7D414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903A4C14-2325-4764-89F3-C6E873CCABE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{364814C2-08EB-4B71-94F0-56459F0CD70F}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>nacionalidade</t>
   </si>
   <si>
-    <t>joia paga</t>
-  </si>
-  <si>
     <t>morada</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>14/5/2021</t>
+  </si>
+  <si>
+    <t>joia paga(TRUE/FALSE)</t>
   </si>
 </sst>
 </file>
@@ -564,9 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1B7D19-0DD8-49AE-8025-B72AC17EA256}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -610,42 +608,42 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="D2" s="2">
         <v>250549361</v>
@@ -654,13 +652,13 @@
         <v>459254851</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="3">
         <v>44079</v>
@@ -669,19 +667,19 @@
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="P2" s="2">
         <v>962681730</v>
@@ -689,13 +687,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D3" s="2">
         <v>250549381</v>
@@ -704,34 +702,34 @@
         <v>459254751</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="J3" s="2" t="b">
         <v>1</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="P3" s="2">
         <v>925827332</v>
@@ -739,20 +737,20 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D4" s="2">
         <v>234517789</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -760,16 +758,16 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="P4" s="2">
         <v>938172388</v>

</xml_diff>